<commit_message>
# Reading pandas dataframe at certain row and col
</commit_message>
<xml_diff>
--- a/pandas.xlsx
+++ b/pandas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gohja\Desktop\excel_data_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B655B0-0D4E-49E7-A162-6AB5BB3A7817}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038A6DA0-F73E-4E45-B556-6143A278A14F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23100" yWindow="2445" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19575" yWindow="2790" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>hey</t>
   </si>
@@ -51,31 +51,7 @@
     <t>zheng</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
+    <t>uF/cm2</t>
   </si>
 </sst>
 </file>
@@ -404,44 +380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="C2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>0</v>
       </c>
@@ -455,7 +402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="5:8" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>4</v>
       </c>
@@ -467,6 +414,71 @@
       </c>
       <c r="H3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>0.60454094899999999</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>0.62367113500000004</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>0.61469258000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>0.605172606</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>0.60945885</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>0.60697734000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>0.62096403300000003</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>0.616542433</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>0.61284272799999995</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>0.60666151199999996</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Added function to read index in Excel file from data passed in from config.json file
</commit_message>
<xml_diff>
--- a/pandas.xlsx
+++ b/pandas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gohja\Desktop\excel_data_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038A6DA0-F73E-4E45-B556-6143A278A14F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64239B30-6D26-48E1-AD77-BA34759BC731}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19575" yWindow="2790" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>hey</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>uF/cm2</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>hry</t>
   </si>
 </sst>
 </file>
@@ -380,15 +389,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:H39"/>
+  <dimension ref="C2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>0</v>
       </c>
@@ -402,7 +411,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="5:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
@@ -416,32 +428,43 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C28">
         <v>0.60454094899999999</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C29">
         <v>0.62367113500000004</v>
       </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C30">
         <v>0.61469258000000004</v>
       </c>
     </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C31">
         <v>0.605172606</v>
       </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C32">
         <v>0.60945885</v>
       </c>
@@ -479,6 +502,11 @@
     <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>